<commit_message>
monthly updates and minor code changes
</commit_message>
<xml_diff>
--- a/data/data_fondos.xlsx
+++ b/data/data_fondos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P900017\Documents\Python Scripts\Tests\web_reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suraperu-my.sharepoint.com/personal/mauricio_meza_sura_pe/Documents/Documents/Python Scripts/Tests/carteras/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8429EEA-234C-47C0-BBF9-5B3B4456511F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{B8429EEA-234C-47C0-BBF9-5B3B4456511F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{21F4BFCA-92AA-4D53-AC65-914EA38541B1}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="CIQWBGuid" hidden="1">"data_fondos.xlsx"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -39,7 +40,7 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_MONTH">15000</definedName>
     <definedName name="IQ_MTD" hidden="1">800000</definedName>
-    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">"05/28/2019 13:29:15"</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">43933.9567361111</definedName>
     <definedName name="IQ_NTM">6000</definedName>
     <definedName name="IQ_QTD" hidden="1">750000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
@@ -1408,7 +1409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>